<commit_message>
Descripción breve de lo que cambiaste
</commit_message>
<xml_diff>
--- a/assets/docs/Maestro_de_Documento.xlsx
+++ b/assets/docs/Maestro_de_Documento.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="124">
   <si>
     <t>Fase</t>
   </si>
@@ -349,10 +349,37 @@
     <t>Documento final 5</t>
   </si>
   <si>
+    <t>Implementacion</t>
+  </si>
+  <si>
+    <t>Plantilla Plan de Implementacion</t>
+  </si>
+  <si>
+    <t>Excel Plan de Pruebas Unitarias</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1FWtU9hSLxstk-De1OQQQcv1uZ_Cow20m/edit?gid=420254295#gid=420254295</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1IbARxuTeOY2qWEzCasl3rCnB_irvc6KH/edit?gid=483070094#gid=483070094</t>
+  </si>
+  <si>
+    <t>Documento Final 6</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1URD1RMH1CQzSUltUoWrTL-RXCT0zOykF/edit?usp=drive_web&amp;ouid=114709403431522966334&amp;rtpof=true</t>
+  </si>
+  <si>
+    <t>Bitacora Individual()</t>
+  </si>
+  <si>
+    <t>Bitacora</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1AM51YULd7YGRPrGdpB-c4GOUy7bbiO_U/edit?rtpof=true</t>
+  </si>
+  <si>
     <t>Bitacora_Tiempo_Nicolas</t>
-  </si>
-  <si>
-    <t>Bitacora</t>
   </si>
   <si>
     <t>https://docs.google.com/document/d/1dvc9DgpfgTd8wvz5caS2-DtgVCq4ESe2/edit</t>
@@ -371,7 +398,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -404,7 +431,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -412,7 +438,14 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -443,47 +476,28 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -755,10 +769,10 @@
       <c r="E2" s="2">
         <v>45881.0</v>
       </c>
-      <c r="F2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -776,10 +790,10 @@
       <c r="E3" s="2">
         <v>45878.0</v>
       </c>
-      <c r="F3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -797,10 +811,10 @@
       <c r="E4" s="2">
         <v>45881.0</v>
       </c>
-      <c r="F4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -815,13 +829,13 @@
       <c r="D5" s="2">
         <v>45881.0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="2">
         <v>45913.0</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>1.1</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -839,10 +853,10 @@
       <c r="E6" s="2">
         <v>45881.0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>1.1</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -860,1182 +874,1228 @@
       <c r="E7" s="2">
         <v>45881.0</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>1.1</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="3">
+      <c r="F10" s="1">
         <v>1.1</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <v>1.2</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="3">
+      <c r="F12" s="1">
         <v>1.2</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="3">
+      <c r="F13" s="1">
         <v>1.2</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G14" s="12" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G15" s="12" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="8" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G16" s="14" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G17" s="12" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G18" s="12" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G19" s="12" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G20" s="12" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G21" s="12" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G22" s="12" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G23" s="12" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G23" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G24" s="12" t="s">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G25" s="12" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G26" s="12" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G27" s="12" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G27" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G28" s="12" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G29" s="12" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G30" s="12" t="s">
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="10"/>
-      <c r="B31" s="11" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G31" s="12" t="s">
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G31" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G32" s="12" t="s">
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11" t="s">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G33" s="10"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11" t="s">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G34" s="10"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="11">
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7">
         <v>1.3</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="11">
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7">
         <v>1.2</v>
       </c>
-      <c r="G36" s="10"/>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11" t="s">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G37" s="12" t="s">
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G37" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11">
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7">
         <v>1.3</v>
       </c>
-      <c r="G38" s="10"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G39" s="12" t="s">
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G39" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G40" s="12" t="s">
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G40" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11" t="s">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="11">
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7">
         <v>1.4</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11" t="s">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="11">
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7">
         <v>1.4</v>
       </c>
-      <c r="G42" s="10"/>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11" t="s">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G43" s="12" t="s">
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11" t="s">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="11">
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7">
         <v>1.4</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="G44" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G45" s="12" t="s">
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G45" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="10"/>
-      <c r="B46" s="11" t="s">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G46" s="10"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11" t="s">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G47" s="10"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="10"/>
-      <c r="B48" s="11" t="s">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G48" s="10"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="10"/>
-      <c r="B49" s="11" t="s">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G49" s="10"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G49" s="7"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="10"/>
-      <c r="B50" s="11" t="s">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G50" s="10"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="10"/>
-      <c r="B51" s="11" t="s">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G51" s="10"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G51" s="7"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="10"/>
-      <c r="B52" s="11" t="s">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="11">
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7">
         <v>1.5</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="G52" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="10"/>
-      <c r="B53" s="11" t="s">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="11">
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7">
         <v>1.5</v>
       </c>
-      <c r="G53" s="10"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="10"/>
-      <c r="B54" s="11" t="s">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G54" s="12" t="s">
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="G54" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="10"/>
-      <c r="B55" s="11" t="s">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="11">
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7">
         <v>1.5</v>
       </c>
-      <c r="G55" s="10"/>
+      <c r="G55" s="7"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
+      <c r="A56" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G56" s="7"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
+      <c r="A57" s="7"/>
+      <c r="B57" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G57" s="7"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
+      <c r="A61" s="7"/>
+      <c r="B61" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="10"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="10"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="10"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="10"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="10"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="10"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10"/>
-      <c r="G74" s="10"/>
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="10"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="10"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="10"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="10"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10"/>
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="10"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="10"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="10"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="10"/>
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="10"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="10"/>
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="10"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="10"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="10"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="10"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="10"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="10"/>
-      <c r="G87" s="10"/>
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="10"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="10"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
+      <c r="A89" s="7"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="10"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="10"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="10"/>
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="10"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="10"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="10"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="10"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="10"/>
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="10"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="10"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="10"/>
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
     </row>
     <row r="98" ht="14.25" customHeight="1"/>
     <row r="99" ht="14.25" customHeight="1"/>
@@ -2977,11 +3037,15 @@
     <hyperlink r:id="rId36" ref="G45"/>
     <hyperlink r:id="rId37" location="gid=1290689837" ref="G52"/>
     <hyperlink r:id="rId38" ref="G54"/>
+    <hyperlink r:id="rId39" location="gid=420254295" ref="G58"/>
+    <hyperlink r:id="rId40" location="gid=483070094" ref="G59"/>
+    <hyperlink r:id="rId41" ref="G60"/>
+    <hyperlink r:id="rId42" ref="G61"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId39"/>
+  <drawing r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -3023,11 +3087,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>110</v>
+      <c r="A2" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2">
         <v>45877.0</v>
@@ -3035,19 +3099,19 @@
       <c r="D2" s="2">
         <v>45881.0</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>1.1</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>112</v>
+      <c r="F2" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>113</v>
+      <c r="A3" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2">
         <v>45877.0</v>
@@ -3055,123 +3119,123 @@
       <c r="D3" s="2">
         <v>45881.0</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>1.1</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>114</v>
+      <c r="F3" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>110</v>
+      <c r="A4" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="15">
+        <v>118</v>
+      </c>
+      <c r="C4" s="11">
         <v>45999.0</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="2">
         <v>45999.0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>1.2</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>112</v>
+      <c r="F4" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>113</v>
+      <c r="A5" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>1.2</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>114</v>
+      <c r="F5" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>110</v>
+      <c r="A6" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="6">
+        <v>118</v>
+      </c>
+      <c r="C6" s="2">
         <v>45894.0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="2">
         <v>45894.0</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>1.3</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>112</v>
+      <c r="F6" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>113</v>
+      <c r="A7" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>1.3</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>114</v>
+      <c r="F7" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>110</v>
+      <c r="A8" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="6">
+        <v>118</v>
+      </c>
+      <c r="C8" s="2">
         <v>45909.0</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="2">
         <v>45909.0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>1.4</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>112</v>
+      <c r="F8" s="12" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>113</v>
+      <c r="A9" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="6">
+        <v>118</v>
+      </c>
+      <c r="C9" s="2">
         <v>45909.0</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="2">
         <v>45909.0</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>1.4</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>114</v>
+      <c r="F9" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Descripcion de tus cambios
</commit_message>
<xml_diff>
--- a/assets/docs/Maestro_de_Documento.xlsx
+++ b/assets/docs/Maestro_de_Documento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="171">
   <si>
     <t>Fase</t>
   </si>
@@ -487,13 +487,55 @@
   </si>
   <si>
     <t>https://docs.google.com/document/d/1E_8H3WSh_a_kwZtwRAoAenqvmkHimTW3/edit</t>
+  </si>
+  <si>
+    <t>Fase 2 Iniciacion/Estrategia</t>
+  </si>
+  <si>
+    <t>Script Iniciacion/Estrategia</t>
+  </si>
+  <si>
+    <t>Script</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1FZeL2aJwuOV36er2c0ukJ75TCr_lW8Su/edit</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1FWtU9hSLxstk-De1OQQQcv1uZ_Cow20m/edit?gid=1810293663#gid=1810293663</t>
+  </si>
+  <si>
+    <t>Informe final Iniciacion/Estrategia</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/15fpu3mqdfj91Iyu9nO-YI6ie_ayGzp_S/edit?slide=id.g39ca7f829a3_0_28#slide=id.g39ca7f829a3_0_28</t>
+  </si>
+  <si>
+    <t>Acta Reunion</t>
+  </si>
+  <si>
+    <t>Acta de reuniones</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/18Khx5feQz3vZF0XRPzZ3xc_DM3NTl3EL/edit</t>
+  </si>
+  <si>
+    <t>Acta de Iniciacion fase 2</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1v43cxT1Jg3MDfaaqG_RAD2kApp7hLz_S/edit</t>
+  </si>
+  <si>
+    <t>Plantilla plan AdminConfiguracion fase 2</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/19E9QiNcSt-NcbuX64onl0LpQWc-pYaUB/edit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -574,6 +616,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -603,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -664,6 +711,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2466,58 +2516,194 @@
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="21"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
+      <c r="A93" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>159</v>
+      </c>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="21"/>
+      <c r="F93" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="G93" s="23" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="21"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="21"/>
+      <c r="B94" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>127</v>
+      </c>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="21"/>
+      <c r="F94" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="G94" s="23" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="21"/>
-      <c r="B95" s="21"/>
-      <c r="C95" s="21"/>
+      <c r="B95" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>18</v>
+      </c>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
-      <c r="F95" s="21"/>
-      <c r="G95" s="21"/>
+      <c r="F95" s="22">
+        <v>1.9</v>
+      </c>
+      <c r="G95" s="13" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="21"/>
-      <c r="B96" s="21"/>
-      <c r="C96" s="21"/>
+      <c r="B96" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>98</v>
+      </c>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
-      <c r="F96" s="21"/>
-      <c r="G96" s="21"/>
+      <c r="F96" s="22">
+        <v>1.9</v>
+      </c>
+      <c r="G96" s="23" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="21"/>
-      <c r="B97" s="21"/>
-      <c r="C97" s="21"/>
+      <c r="B97" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>147</v>
+      </c>
       <c r="D97" s="21"/>
       <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="21"/>
-    </row>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
+      <c r="F97" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="G97" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="98" ht="14.25" customHeight="1">
+      <c r="A98" s="21"/>
+      <c r="B98" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D98" s="21"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="22">
+        <v>1.1</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="99" ht="14.25" customHeight="1">
+      <c r="A99" s="21"/>
+      <c r="B99" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C99" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="22">
+        <v>1.1</v>
+      </c>
+      <c r="G99" s="23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="100" ht="14.25" customHeight="1">
+      <c r="A100" s="21"/>
+      <c r="B100" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
+      <c r="F100" s="22">
+        <v>1.1</v>
+      </c>
+      <c r="G100" s="24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="101" ht="14.25" customHeight="1">
+      <c r="A101" s="21"/>
+      <c r="B101" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="22">
+        <v>1.9</v>
+      </c>
+      <c r="G101" s="21"/>
+    </row>
+    <row r="102" ht="14.25" customHeight="1">
+      <c r="A102" s="21"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="21"/>
+      <c r="E102" s="21"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="21"/>
+    </row>
+    <row r="103" ht="14.25" customHeight="1">
+      <c r="A103" s="21"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="21"/>
+    </row>
+    <row r="104" ht="14.25" customHeight="1">
+      <c r="A104" s="21"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="21"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="21"/>
+    </row>
+    <row r="105" ht="14.25" customHeight="1">
+      <c r="A105" s="21"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="21"/>
+      <c r="D105" s="21"/>
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="21"/>
+    </row>
     <row r="106" ht="14.25" customHeight="1"/>
     <row r="107" ht="14.25" customHeight="1"/>
     <row r="108" ht="14.25" customHeight="1"/>
@@ -3485,10 +3671,18 @@
     <hyperlink r:id="rId71" ref="G90"/>
     <hyperlink r:id="rId72" ref="G91"/>
     <hyperlink r:id="rId73" ref="G92"/>
+    <hyperlink r:id="rId74" ref="G93"/>
+    <hyperlink r:id="rId75" ref="G94"/>
+    <hyperlink r:id="rId76" location="gid=483070094" ref="G95"/>
+    <hyperlink r:id="rId77" location="gid=1810293663" ref="G96"/>
+    <hyperlink r:id="rId78" location="slide=id.g39ca7f829a3_0_28" ref="G97"/>
+    <hyperlink r:id="rId79" ref="G98"/>
+    <hyperlink r:id="rId80" ref="G99"/>
+    <hyperlink r:id="rId81" ref="G100"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId74"/>
+  <drawing r:id="rId82"/>
 </worksheet>
 </file>
</xml_diff>